<commit_message>
Worked on 144 G100 Black roman & italic, updated recipes with new master names
</commit_message>
<xml_diff>
--- a/sources/ScaleAndInterpolate Recipes.xlsx
+++ b/sources/ScaleAndInterpolate Recipes.xlsx
@@ -26,12 +26,12 @@
     <t>Kerning</t>
   </si>
   <si>
-    <t>Black OpMax GoofyMax 
+    <t>144G100Black 
 (Roman &amp; Italic)</t>
   </si>
   <si>
-    <t>Light OpMin GoofyMax + 
-Black OpMin GoofyMax</t>
+    <t>9G100Light + 
+9G100Black</t>
   </si>
   <si>
     <t>Caps
@@ -52,7 +52,7 @@
     <t>Start by interpolating with ScaleAndInterpolate.py</t>
   </si>
   <si>
-    <t>Light OpMax GoofyMax 
+    <t>144G100Light
 (Roman &amp; Italic)</t>
   </si>
   <si>
@@ -71,15 +71,15 @@
 Skew: 2° (italic only)</t>
   </si>
   <si>
-    <t>Start by copying from Light OpMax GoofyMin</t>
-  </si>
-  <si>
-    <t>Black OpMin GoofyMin 
+    <t>Start by copying from 144G0Light</t>
+  </si>
+  <si>
+    <t>9G0Black 
 (Roman &amp; Italic)</t>
   </si>
   <si>
-    <t>Black OpMax GoofyMin + 
-Black OpMin GoofyMax</t>
+    <t>144G0Black + 
+9G100Black</t>
   </si>
   <si>
     <t>Caps
@@ -97,15 +97,15 @@
 Skew: 0°</t>
   </si>
   <si>
-    <t>Copy from Black OpMin GoofyMax, will only need minor adjustments</t>
-  </si>
-  <si>
-    <t>Light OpMin GoofyMin 
+    <t>Copy from 9G100Black, will only need minor adjustments</t>
+  </si>
+  <si>
+    <t>9G0Light 
 (Roman &amp; Italic)</t>
   </si>
   <si>
-    <t>Light OpMax GoofyMin + 
-Light OpMin GoofyMax</t>
+    <t>144G0Light + 
+9G100Light</t>
   </si>
   <si>
     <t>Caps
@@ -123,7 +123,7 @@
 Skew: 0°</t>
   </si>
   <si>
-    <t>Copy from Light OpMin GoofyMax, will only need minor adjustments</t>
+    <t>Copy from 9G100Light, will only need minor adjustments</t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -141,6 +141,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -156,15 +161,21 @@
       <name val="Menlo"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -174,16 +185,116 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -193,17 +304,47 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -223,7 +364,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -240,10 +383,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -420,11 +563,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -433,27 +579,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -710,10 +856,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1004,7 +1150,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1285,17 +1431,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.6328" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6328" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.2109" style="1" customWidth="1"/>
-    <col min="4" max="4" width="78.7109" style="1" customWidth="1"/>
-    <col min="5" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="78.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.35" customHeight="1">
@@ -1311,62 +1458,102 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="173.35" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="4">
         <v>7</v>
       </c>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" ht="173.35" customHeight="1">
-      <c r="A3" t="s" s="3">
+      <c r="A3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" t="s" s="4">
         <v>10</v>
       </c>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" ht="184.35" customHeight="1">
-      <c r="A4" t="s" s="3">
+      <c r="A4" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" t="s" s="4">
         <v>14</v>
       </c>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" ht="173.35" customHeight="1">
-      <c r="A5" t="s" s="3">
+      <c r="A5" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B5" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C5" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="3">
+      <c r="D5" t="s" s="4">
         <v>18</v>
       </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>